<commit_message>
make some reminder tokens be global
</commit_message>
<xml_diff>
--- a/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
+++ b/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\botc\botc_other\all_hat_and_no_cattle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FD049C-30AF-44B6-BACE-DC67701A0676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75612B3C-633B-4B21-89D8-59B70A9A9A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="98">
   <si>
     <t>All Hat And No Cattle</t>
   </si>
@@ -154,163 +154,166 @@
     <t>Cotillion</t>
   </si>
   <si>
+    <t>No ability</t>
+  </si>
+  <si>
+    <t>Ability (each night).</t>
+  </si>
+  <si>
+    <t>Hox</t>
+  </si>
+  <si>
+    <t>Messiah</t>
+  </si>
+  <si>
+    <t>Once per game, when you are dead, if you are executed you come back to life.</t>
+  </si>
+  <si>
+    <t>Ability (once per game).</t>
+  </si>
+  <si>
+    <t>Satirist</t>
+  </si>
+  <si>
+    <t>The first time you are chosen at night by an evil character (not travelers), you learn which. Their ability is redirected (without warning) at a new target of your choice.</t>
+  </si>
+  <si>
+    <t>Hermit</t>
+  </si>
+  <si>
+    <t>If only one good player is left alive, you learn the demon bluffs before you wake.</t>
+  </si>
+  <si>
+    <t>Any player (not yourself) who votes when you are nominated cannot die tonight, and one is drunk tonight.</t>
+  </si>
+  <si>
+    <t>Protected, Drunk</t>
+  </si>
+  <si>
+    <t>Apatheist</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Jailer</t>
+  </si>
+  <si>
+    <t>outsider</t>
+  </si>
+  <si>
+    <t>If one/both of their picks died since last night, tell them this.</t>
+  </si>
+  <si>
+    <t>Brewer</t>
+  </si>
+  <si>
+    <t>You think you are a different character. One of your neighbours cannot die, the other is drunk.</t>
+  </si>
+  <si>
+    <t>Is the Brewer, Drunk, Protected</t>
+  </si>
+  <si>
+    <t>Return character type count (night 2).</t>
+  </si>
+  <si>
+    <t>You might start evil. If you die at night, choose a player (not yourself). You switch to their alignment and then die.</t>
+  </si>
+  <si>
+    <t>If they are the only good player alive, tell them the demon bluffs.</t>
+  </si>
+  <si>
+    <t>If a player is nominated and executed and you did not vote on their nomination, something bad might happen to your team. You survive execution.</t>
+  </si>
+  <si>
+    <t>Something bad</t>
+  </si>
+  <si>
+    <t>Lemming</t>
+  </si>
+  <si>
+    <t>If a Lemming dies, so do all other Lemmings. When Lemmings die, a dead minion regains their ability.</t>
+  </si>
+  <si>
+    <t>Has ability</t>
+  </si>
+  <si>
+    <t>minion</t>
+  </si>
+  <si>
+    <t>Each night, choose a player (different to last night). You learn their character and control any choices they make tonight. (They learn these choices.)</t>
+  </si>
+  <si>
+    <t>Each night, if there were more dead than living players at dusk, choose a dead player, their ghost vote is removed.</t>
+  </si>
+  <si>
+    <t>Remove vote</t>
+  </si>
+  <si>
+    <t>On your first night, choose clockwise or anticlockwise. Twice per game, at night*, along neighbouring alive players in that direction, choose if the furthest from you dies.</t>
+  </si>
+  <si>
+    <t>Clockwise, Anticlockwise, Shot once, No ability, Dead</t>
+  </si>
+  <si>
+    <t>Siren</t>
+  </si>
+  <si>
+    <t>Each time you are nominated by an opposing player, they become drunk, even if you are dead.</t>
+  </si>
+  <si>
+    <t>demon</t>
+  </si>
+  <si>
+    <t>Each night*, choose a player to die. One of your minions has a non-listed (minion) role. A good player might learn which non-listed role is in play, if so the minion learns who.</t>
+  </si>
+  <si>
+    <t>Dead, Learned, Non-listed minion</t>
+  </si>
+  <si>
+    <t>Each night*, either: choose a player to become a Lemming, or choose a player to die. [+0 or +1 outsiders]</t>
+  </si>
+  <si>
+    <t>Dead</t>
+  </si>
+  <si>
+    <t>You see the Grimoire on your first night. Each night*, choose a neighbour of an already dead player to die, even if they might have survived for some reason. (Or anyone if all players live.)</t>
+  </si>
+  <si>
+    <t>traveler</t>
+  </si>
+  <si>
+    <t>Pollster</t>
+  </si>
+  <si>
+    <t>When you are nominated, or your exile is called for, visit the storyteller privately and choose a number. If exactly that many players vote, you win.</t>
+  </si>
+  <si>
+    <t>Each night*, choose a player, they are placed on the block at dawn.</t>
+  </si>
+  <si>
+    <t>On the block</t>
+  </si>
+  <si>
+    <t>Triffid</t>
+  </si>
+  <si>
+    <t>On a tied nomination vote, both (or more) players are placed on the block. If so, at the end of the day, you choose if they are (all) executed.</t>
+  </si>
+  <si>
+    <t>When a good player is targeted by an evil players ability, the ability malfunctions. Instead, the good player aligns with and learns the evil player; even if you are drunk or dead. [There are two evil teams.]</t>
+  </si>
+  <si>
+    <t>Once per game, at night, choose an alive player (not yourself). They are woken and asked to choose a character. That character wakes to learn that the Messenger is in play.</t>
+  </si>
+  <si>
+    <t>Each night*, choose a player to die. If you choose yourself then (after your death) a good player turns into an evil Hox and you become good. You don't learn bluffs or minions. Minions know (only) you and learn bluffs. [+1 minion]</t>
+  </si>
+  <si>
     <t>Once per game, at night, choose a player. If you choose a player of the same alignment or a demon, nothing happens. Otherwise, swap characters.</t>
   </si>
   <si>
-    <t>No ability</t>
-  </si>
-  <si>
-    <t>Ability (each night).</t>
-  </si>
-  <si>
-    <t>Hox</t>
-  </si>
-  <si>
-    <t>Messiah</t>
-  </si>
-  <si>
-    <t>Once per game, when you are dead, if you are executed you come back to life.</t>
-  </si>
-  <si>
-    <t>Ability (once per game).</t>
-  </si>
-  <si>
-    <t>Satirist</t>
-  </si>
-  <si>
-    <t>The first time you are chosen at night by an evil character (not travelers), you learn which. Their ability is redirected (without warning) at a new target of your choice.</t>
-  </si>
-  <si>
-    <t>Hermit</t>
-  </si>
-  <si>
-    <t>If only one good player is left alive, you learn the demon bluffs before you wake.</t>
-  </si>
-  <si>
-    <t>Any player (not yourself) who votes when you are nominated cannot die tonight, and one is drunk tonight.</t>
-  </si>
-  <si>
-    <t>Protected, Drunk</t>
-  </si>
-  <si>
-    <t>Apatheist</t>
-  </si>
-  <si>
-    <t>Team</t>
-  </si>
-  <si>
-    <t>Jailer</t>
-  </si>
-  <si>
-    <t>outsider</t>
-  </si>
-  <si>
-    <t>If one/both of their picks died since last night, tell them this.</t>
-  </si>
-  <si>
-    <t>Brewer</t>
-  </si>
-  <si>
-    <t>You think you are a different character. One of your neighbours cannot die, the other is drunk.</t>
-  </si>
-  <si>
-    <t>Is the Brewer, Drunk, Protected</t>
-  </si>
-  <si>
-    <t>Return character type count (night 2).</t>
-  </si>
-  <si>
-    <t>You might start evil. If you die at night, choose a player (not yourself). You switch to their alignment and then die.</t>
-  </si>
-  <si>
-    <t>If they are the only good player alive, tell them the demon bluffs.</t>
-  </si>
-  <si>
-    <t>If a player is nominated and executed and you did not vote on their nomination, something bad might happen to your team. You survive execution.</t>
-  </si>
-  <si>
-    <t>Something bad</t>
-  </si>
-  <si>
-    <t>Lemming</t>
-  </si>
-  <si>
-    <t>If a Lemming dies, so do all other Lemmings. When Lemmings die, a dead minion regains their ability.</t>
-  </si>
-  <si>
-    <t>Has ability</t>
-  </si>
-  <si>
-    <t>minion</t>
-  </si>
-  <si>
-    <t>Each night, choose a player (different to last night). You learn their character and control any choices they make tonight. (They learn these choices.)</t>
-  </si>
-  <si>
-    <t>Each night, if there were more dead than living players at dusk, choose a dead player, their ghost vote is removed.</t>
-  </si>
-  <si>
-    <t>Remove vote</t>
-  </si>
-  <si>
-    <t>On your first night, choose clockwise or anticlockwise. Twice per game, at night*, along neighbouring alive players in that direction, choose if the furthest from you dies.</t>
-  </si>
-  <si>
-    <t>Clockwise, Anticlockwise, Shot once, No ability, Dead</t>
-  </si>
-  <si>
-    <t>Siren</t>
-  </si>
-  <si>
-    <t>Each time you are nominated by an opposing player, they become drunk, even if you are dead.</t>
-  </si>
-  <si>
-    <t>demon</t>
-  </si>
-  <si>
-    <t>Each night*, choose a player to die. One of your minions has a non-listed (minion) role. A good player might learn which non-listed role is in play, if so the minion learns who.</t>
-  </si>
-  <si>
-    <t>Dead, Learned, Non-listed minion</t>
-  </si>
-  <si>
-    <t>Each night*, either: choose a player to become a Lemming, or choose a player to die. [+0 or +1 outsiders]</t>
-  </si>
-  <si>
-    <t>Dead</t>
-  </si>
-  <si>
-    <t>You see the Grimoire on your first night. Each night*, choose a neighbour of an already dead player to die, even if they might have survived for some reason. (Or anyone if all players live.)</t>
-  </si>
-  <si>
-    <t>traveler</t>
-  </si>
-  <si>
-    <t>Pollster</t>
-  </si>
-  <si>
-    <t>When you are nominated, or your exile is called for, visit the storyteller privately and choose a number. If exactly that many players vote, you win.</t>
-  </si>
-  <si>
-    <t>Each night*, choose a player, they are placed on the block at dawn.</t>
-  </si>
-  <si>
-    <t>On the block</t>
-  </si>
-  <si>
-    <t>Triffid</t>
-  </si>
-  <si>
-    <t>On a tied nomination vote, both (or more) players are placed on the block. If so, at the end of the day, you choose if they are (all) executed.</t>
-  </si>
-  <si>
-    <t>When a good player is targeted by an evil players ability, the ability malfunctions. Instead, the good player aligns with and learns the evil player; even if you are drunk or dead. [There are two evil teams.]</t>
-  </si>
-  <si>
-    <t>Once per game, at night, choose an alive player (not yourself). They are woken and asked to choose a character. That character wakes to learn that the Messenger is in play.</t>
-  </si>
-  <si>
-    <t>Each night*, choose a player to die. If you choose yourself then (after your death) a good player turns into an evil Hox and you become good. You don't learn bluffs or minions. Minions know (only) you and learn bluffs. [+1 minion]</t>
+    <t>Global Reminders</t>
   </si>
 </sst>
 </file>
@@ -1151,25 +1154,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="200.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="4" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1177,47 +1180,50 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>11</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -1227,46 +1233,46 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
         <v>22</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>16</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>24</v>
       </c>
@@ -1276,46 +1282,46 @@
       <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>27</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>28</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>29</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>31</v>
       </c>
       <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>33</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>22</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>34</v>
       </c>
@@ -1325,23 +1331,23 @@
       <c r="D9" t="s">
         <v>36</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
         <v>37</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>38</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>39</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>40</v>
       </c>
@@ -1351,407 +1357,407 @@
       <c r="D10" t="s">
         <v>36</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
         <v>42</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>38</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>43</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>42</v>
       </c>
       <c r="C11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" t="s">
         <v>44</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
         <v>45</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>27</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>47</v>
       </c>
-      <c r="I12" t="s">
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>37</v>
-      </c>
-      <c r="I14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
         <v>55</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>56</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>59</v>
       </c>
-      <c r="I17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="I18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" t="s">
         <v>60</v>
       </c>
-      <c r="H18" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" t="s">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>62</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>63</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" t="s">
         <v>64</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" t="s">
         <v>66</v>
       </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="H20" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>18</v>
       </c>
       <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
         <v>68</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>69</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>70</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>71</v>
       </c>
-      <c r="D22" t="s">
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>72</v>
       </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>29</v>
       </c>
       <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" t="s">
         <v>75</v>
       </c>
-      <c r="D25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>22</v>
       </c>
       <c r="C26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" t="s">
         <v>77</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>78</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>79</v>
-      </c>
-      <c r="C27" t="s">
-        <v>80</v>
       </c>
       <c r="D27" t="s">
         <v>15</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>39</v>
       </c>
       <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" t="s">
         <v>82</v>
       </c>
-      <c r="D29" t="s">
-        <v>83</v>
-      </c>
-      <c r="E29">
+      <c r="F29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>43</v>
       </c>
       <c r="C30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" t="s">
         <v>84</v>
       </c>
-      <c r="D30" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30">
+      <c r="F30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>27</v>
       </c>
       <c r="C31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>86</v>
       </c>
-      <c r="D31" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" t="s">
-        <v>85</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>88</v>
       </c>
-      <c r="C34" t="s">
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" t="s">
         <v>89</v>
       </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>90</v>
       </c>
-      <c r="D35" t="s">
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>91</v>
       </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>92</v>
       </c>
-      <c r="C36" t="s">
-        <v>93</v>
-      </c>
       <c r="D36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36">
+        <v>90</v>
+      </c>
+      <c r="F36">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add date, reword satirist
</commit_message>
<xml_diff>
--- a/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
+++ b/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\botc\botc_other\all_hat_and_no_cattle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AA7C20-48EA-41DD-BCDC-323222F054D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47F9AC4-58BA-4C89-8FA8-C92139DA4DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,9 +55,6 @@
     <t>Guard</t>
   </si>
   <si>
-    <t>Mark protected players.</t>
-  </si>
-  <si>
     <t>Understudy</t>
   </si>
   <si>
@@ -292,9 +289,6 @@
     <t>On a tied nomination vote, both (or more) players are placed on the block. If so, at the end of the day, you choose if they are (all) executed.</t>
   </si>
   <si>
-    <t>When a good player is targeted by an evil players ability, the ability malfunctions. Instead, the good player aligns with and learns the evil player; even if you are drunk or dead. [There are two evil teams.]</t>
-  </si>
-  <si>
     <t>Once per game, at night, choose an alive player (not yourself). They are woken and asked to choose a character. That character wakes to learn that the Messenger is in play.</t>
   </si>
   <si>
@@ -313,7 +307,13 @@
     <t>Mark if something bad could happen tonight.</t>
   </si>
   <si>
-    <t>The first time you are chosen at night by an evil character (not travelers), you learn which. Their ability is redirected (without warning) at a new target of your choice.</t>
+    <t>Mark protected &amp; drunk players.</t>
+  </si>
+  <si>
+    <t>The first time you are chosen at night by a minions ability, it malfunctions. You learn which ability and you gain that ability tonight.</t>
+  </si>
+  <si>
+    <t>When a good player is chosen at night by an evil players ability, it malfunctions. Instead, the good player aligns with and learns the evil player; even if you are drunk or dead. [There are two evil teams.]</t>
   </si>
 </sst>
 </file>
@@ -1156,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1214,96 +1214,96 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
       <c r="J5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
         <v>19</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>20</v>
       </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
       <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
         <v>15</v>
-      </c>
-      <c r="J6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>24</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>25</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>26</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>27</v>
-      </c>
-      <c r="J7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
         <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1312,168 +1312,168 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
         <v>34</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>35</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>36</v>
       </c>
-      <c r="I9" t="s">
-        <v>37</v>
-      </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
         <v>40</v>
       </c>
-      <c r="H10" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" t="s">
-        <v>41</v>
-      </c>
       <c r="J10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
         <v>42</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" t="s">
-        <v>43</v>
-      </c>
       <c r="I11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
         <v>45</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" t="s">
         <v>46</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="I13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
         <v>49</v>
       </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1481,70 +1481,70 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
         <v>51</v>
       </c>
-      <c r="D16" t="s">
-        <v>52</v>
-      </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" t="s">
         <v>53</v>
-      </c>
-      <c r="C17" t="s">
-        <v>90</v>
-      </c>
-      <c r="E17" t="s">
-        <v>54</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" t="s">
         <v>56</v>
-      </c>
-      <c r="I18" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
         <v>58</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>59</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" t="s">
         <v>60</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>38</v>
-      </c>
-      <c r="J19" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1552,47 +1552,47 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
         <v>64</v>
       </c>
-      <c r="D21" t="s">
-        <v>65</v>
-      </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
         <v>66</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>67</v>
-      </c>
-      <c r="D22" t="s">
-        <v>68</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1600,15 +1600,15 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
         <v>71</v>
-      </c>
-      <c r="D25" t="s">
-        <v>72</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
         <v>73</v>
-      </c>
-      <c r="D26" t="s">
-        <v>74</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
         <v>75</v>
       </c>
-      <c r="C27" t="s">
-        <v>76</v>
-      </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1658,18 +1658,18 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" t="s">
         <v>78</v>
-      </c>
-      <c r="D29" t="s">
-        <v>79</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1677,13 +1677,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" t="s">
         <v>80</v>
-      </c>
-      <c r="D30" t="s">
-        <v>81</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1691,13 +1691,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1705,13 +1705,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1719,15 +1719,15 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" t="s">
         <v>84</v>
-      </c>
-      <c r="C34" t="s">
-        <v>85</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1735,13 +1735,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" t="s">
         <v>86</v>
-      </c>
-      <c r="D35" t="s">
-        <v>87</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1749,13 +1749,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" t="s">
         <v>88</v>
       </c>
-      <c r="C36" t="s">
-        <v>89</v>
-      </c>
       <c r="D36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F36">
         <v>0</v>

</xml_diff>

<commit_message>
hox chooses alive players
</commit_message>
<xml_diff>
--- a/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
+++ b/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\botc\botc_other\all_hat_and_no_cattle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09671EE-906E-4A71-8618-9E743D05A068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF51910A-D102-4A2D-A361-1F6DAF4BFE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -322,7 +322,7 @@
     <t>Each day, visit the storyteller and answer a yes/no question. In return you receive a piece of information, which is true if you answered correctly.</t>
   </si>
   <si>
-    <t>Each night*, choose a player to die. If you choose yourself then (after your death) a good player turns into an evil Hox and you become good. You don't learn bluffs or minions. Minions know you and learn bluffs. [+1 Outsider]</t>
+    <t>Each night*, choose a player to die. If you choose yourself then (after your death) an alive good player turns into an evil Hox and you become good. You don't learn bluffs or minions. Minions know you and learn bluffs. [+1 Outsider]</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
potato does not choose travellers
</commit_message>
<xml_diff>
--- a/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
+++ b/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\botc\botc_other\all_hat_and_no_cattle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405F820E-2E9A-4436-A469-EF2C5D0B244A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961A2BA6-179F-47C2-A322-BA6E36EF8BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,9 +232,6 @@
     <t>Once per game, at night, choose an alive player (not yourself). They are woken and asked to choose a character. That character wakes to learn that the Messenger is in play.</t>
   </si>
   <si>
-    <t>Once per game, at night, choose a player. If you choose a player of the same alignment or a demon, nothing happens. Otherwise, swap characters.</t>
-  </si>
-  <si>
     <t>Global Reminders</t>
   </si>
   <si>
@@ -323,6 +320,9 @@
   </si>
   <si>
     <t>On your first night, choose clockwise or anticlockwise. Once per game, at night*, along neighbouring alive players in that direction, choose if the furthest two from you die. The demon is drunk that night.</t>
+  </si>
+  <si>
+    <t>Once per game, at night, choose a player (not travelers). If you choose a player of the same alignment or a demon, nothing happens. Otherwise, swap characters.</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1166,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1223,13 +1223,13 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1249,13 +1249,13 @@
         <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I5" t="s">
         <v>35</v>
       </c>
       <c r="J5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1278,7 +1278,7 @@
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1298,13 +1298,13 @@
         <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I7" t="s">
         <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1312,7 +1312,7 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1321,13 +1321,13 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I8" t="s">
         <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1335,7 +1335,7 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
@@ -1347,13 +1347,13 @@
         <v>28</v>
       </c>
       <c r="H9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
       </c>
       <c r="J9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1373,13 +1373,13 @@
         <v>31</v>
       </c>
       <c r="H10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1387,7 +1387,7 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="D11" t="s">
         <v>33</v>
@@ -1399,13 +1399,13 @@
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I11" t="s">
         <v>32</v>
       </c>
       <c r="J11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1425,7 +1425,7 @@
         <v>23</v>
       </c>
       <c r="J12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1433,7 +1433,7 @@
         <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1442,7 +1442,7 @@
         <v>34</v>
       </c>
       <c r="J13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1450,7 +1450,7 @@
         <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -1462,7 +1462,7 @@
         <v>31</v>
       </c>
       <c r="J14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1479,7 +1479,7 @@
         <v>28</v>
       </c>
       <c r="J15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1487,10 +1487,10 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1499,7 +1499,7 @@
         <v>11</v>
       </c>
       <c r="J16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1507,7 +1507,7 @@
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
         <v>40</v>
@@ -1519,7 +1519,7 @@
         <v>16</v>
       </c>
       <c r="J17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1530,7 +1530,7 @@
         <v>41</v>
       </c>
       <c r="J18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1541,7 +1541,7 @@
         <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1575,7 +1575,7 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
         <v>49</v>
@@ -1595,7 +1595,7 @@
         <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
         <v>51</v>
@@ -1607,7 +1607,7 @@
         <v>20</v>
       </c>
       <c r="J22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1620,7 +1620,7 @@
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1645,10 +1645,10 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1675,10 +1675,10 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
         <v>58</v>
@@ -1692,7 +1692,7 @@
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
         <v>59</v>
@@ -1706,7 +1706,7 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D31" t="s">
         <v>59</v>
@@ -1720,7 +1720,7 @@
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D32" t="s">
         <v>59</v>
@@ -1739,7 +1739,7 @@
         <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1764,7 +1764,7 @@
         <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D36" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
add some more reminder tokens & fix vizier night order
</commit_message>
<xml_diff>
--- a/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
+++ b/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\botc\botc_other\all_hat_and_no_cattle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961A2BA6-179F-47C2-A322-BA6E36EF8BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43F6ABA-2A8F-4821-9263-63024263A527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1166,7 +1166,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
sorting hat does not choose travellers
</commit_message>
<xml_diff>
--- a/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
+++ b/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\botc\botc_other\all_hat_and_no_cattle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43F6ABA-2A8F-4821-9263-63024263A527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159EFE6D-0DA0-415D-9B5B-73B77912D62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="99">
   <si>
     <t>All Hat And No Cattle</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Sorting Hat</t>
   </si>
   <si>
-    <t>On your first day, publicly choose 4 players (not yourself). At night you learn how many different character types they were.</t>
-  </si>
-  <si>
     <t>Potato</t>
   </si>
   <si>
@@ -323,6 +320,15 @@
   </si>
   <si>
     <t>Once per game, at night, choose a player (not travelers). If you choose a player of the same alignment or a demon, nothing happens. Otherwise, swap characters.</t>
+  </si>
+  <si>
+    <t>Hypnotized, Choice</t>
+  </si>
+  <si>
+    <t>Chosen, Died</t>
+  </si>
+  <si>
+    <t>On your first day, publicly choose 4 players (not yourself or travelers). At night you learn how many different character types they were.</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1172,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1195,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1223,13 +1229,13 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1249,13 +1255,13 @@
         <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1278,7 +1284,7 @@
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1298,13 +1304,13 @@
         <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I7" t="s">
         <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1312,7 +1318,7 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1321,13 +1327,13 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I8" t="s">
         <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1335,10 +1341,10 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1347,13 +1353,13 @@
         <v>28</v>
       </c>
       <c r="H9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
       </c>
       <c r="J9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1361,7 +1367,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
@@ -1370,27 +1376,27 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1399,13 +1405,13 @@
         <v>11</v>
       </c>
       <c r="H11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" t="s">
         <v>77</v>
-      </c>
-      <c r="I11" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1413,10 +1419,10 @@
         <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1425,52 +1431,52 @@
         <v>23</v>
       </c>
       <c r="J12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1479,7 +1485,7 @@
         <v>28</v>
       </c>
       <c r="J15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1487,10 +1493,10 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1499,18 +1505,18 @@
         <v>11</v>
       </c>
       <c r="J16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
         <v>39</v>
-      </c>
-      <c r="C17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" t="s">
-        <v>40</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1519,29 +1525,29 @@
         <v>16</v>
       </c>
       <c r="J17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
         <v>44</v>
       </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1550,7 +1556,7 @@
         <v>26</v>
       </c>
       <c r="J19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1558,7 +1564,7 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1567,7 +1573,7 @@
         <v>29</v>
       </c>
       <c r="J20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1575,30 +1581,30 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" t="s">
         <v>50</v>
-      </c>
-      <c r="C22" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" t="s">
-        <v>51</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1607,12 +1613,12 @@
         <v>20</v>
       </c>
       <c r="J22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1620,7 +1626,10 @@
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="D24" t="s">
+        <v>96</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1631,10 +1640,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
         <v>53</v>
-      </c>
-      <c r="D25" t="s">
-        <v>54</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1645,10 +1654,10 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1656,10 +1665,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
         <v>55</v>
-      </c>
-      <c r="C27" t="s">
-        <v>56</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
@@ -1670,18 +1679,18 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1689,13 +1698,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1706,10 +1715,10 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1717,13 +1726,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1731,15 +1740,15 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1747,13 +1756,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" t="s">
         <v>62</v>
-      </c>
-      <c r="D35" t="s">
-        <v>63</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1761,13 +1770,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F36">
         <v>0</v>

</xml_diff>

<commit_message>
pollster, hox & hermit: ability changes
</commit_message>
<xml_diff>
--- a/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
+++ b/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\botc\botc_other\all_hat_and_no_cattle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159EFE6D-0DA0-415D-9B5B-73B77912D62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AD12F6-0901-455D-B5E4-1C1B8C0B1EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="All Hat And No Cattle" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -145,9 +146,6 @@
     <t>Hermit</t>
   </si>
   <si>
-    <t>If only one good player is left alive, you learn the demon bluffs before you wake.</t>
-  </si>
-  <si>
     <t>Apatheist</t>
   </si>
   <si>
@@ -274,15 +272,9 @@
     <t>Ability - first night.</t>
   </si>
   <si>
-    <t xml:space="preserve">If a Lemming dies, so do all other Lemmings. When Lemmings die, a dead minion might regain their ability for one day and night. </t>
-  </si>
-  <si>
     <t>Any player (not yourself) who votes when you are nominated cannot die tonight, and one is drunk tonight.</t>
   </si>
   <si>
-    <t>When your exile is called for, visit the storyteller privately and choose a number. If exactly that many players vote, you win.</t>
-  </si>
-  <si>
     <t>On a tied nomination vote, two (or more) players are placed on the block. If so, at the end of the day, you choose which one of them is executed.</t>
   </si>
   <si>
@@ -313,9 +305,6 @@
     <t>Each day, visit the storyteller and answer a yes/no question. In return you receive a piece of information, which is true if you answered correctly.</t>
   </si>
   <si>
-    <t>Each night*, choose a player to die. If you choose yourself then (after your death) an alive good player turns into an evil Hox and you become good. You don't learn bluffs or minions. Minions know you and learn bluffs. [+1 Outsider]</t>
-  </si>
-  <si>
     <t>On your first night, choose clockwise or anticlockwise. Once per game, at night*, along neighbouring alive players in that direction, choose if the furthest two from you die. The demon is drunk that night.</t>
   </si>
   <si>
@@ -329,6 +318,18 @@
   </si>
   <si>
     <t>On your first day, publicly choose 4 players (not yourself or travelers). At night you learn how many different character types they were.</t>
+  </si>
+  <si>
+    <t>When your exile is called for, visit the storyteller privately and choose a number. If exactly that many players vote, everyone who voted dies.</t>
+  </si>
+  <si>
+    <t>The first time only one good player is alive at dawn, you wake and choose a player to come back to life.</t>
+  </si>
+  <si>
+    <t>If a Lemming dies, so do all other Lemmings. When Lemmings die, a dead minion might regain their ability for one day and night.</t>
+  </si>
+  <si>
+    <t>Each night*, choose a player to die. If you choose yourself then (after your death) minions wake to choose a new evil hox and you become good. You don't learn bluffs or minions. Minions know you and learn bluffs. [+1 Outsider]</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1173,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1229,13 +1230,13 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1255,13 +1256,13 @@
         <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I5" t="s">
         <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1284,7 +1285,7 @@
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1304,13 +1305,13 @@
         <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I7" t="s">
         <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1318,7 +1319,7 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1327,13 +1328,13 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I8" t="s">
         <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1341,10 +1342,10 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1353,13 +1354,13 @@
         <v>28</v>
       </c>
       <c r="H9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
       </c>
       <c r="J9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1367,7 +1368,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
@@ -1379,13 +1380,13 @@
         <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1393,7 +1394,7 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
@@ -1405,13 +1406,13 @@
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I11" t="s">
         <v>31</v>
       </c>
       <c r="J11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1419,7 +1420,7 @@
         <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -1431,7 +1432,7 @@
         <v>23</v>
       </c>
       <c r="J12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1439,7 +1440,7 @@
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1448,7 +1449,7 @@
         <v>33</v>
       </c>
       <c r="J13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1456,7 +1457,7 @@
         <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D14" t="s">
         <v>32</v>
@@ -1468,7 +1469,7 @@
         <v>30</v>
       </c>
       <c r="J14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1476,7 +1477,7 @@
         <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1485,7 +1486,7 @@
         <v>28</v>
       </c>
       <c r="J15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1493,10 +1494,10 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1505,18 +1506,18 @@
         <v>11</v>
       </c>
       <c r="J16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" t="s">
         <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" t="s">
-        <v>39</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1525,29 +1526,29 @@
         <v>16</v>
       </c>
       <c r="J17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
         <v>43</v>
       </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1556,7 +1557,7 @@
         <v>26</v>
       </c>
       <c r="J19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1564,7 +1565,7 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1573,7 +1574,7 @@
         <v>29</v>
       </c>
       <c r="J20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1581,10 +1582,10 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1593,18 +1594,18 @@
         <v>36</v>
       </c>
       <c r="J21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" t="s">
         <v>49</v>
-      </c>
-      <c r="C22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" t="s">
-        <v>50</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1613,12 +1614,12 @@
         <v>20</v>
       </c>
       <c r="J22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1626,10 +1627,10 @@
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D24" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1640,10 +1641,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
         <v>52</v>
-      </c>
-      <c r="D25" t="s">
-        <v>53</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1654,10 +1655,10 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1665,10 +1666,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
         <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>55</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
@@ -1679,18 +1680,18 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1701,10 +1702,10 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1715,10 +1716,10 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1729,10 +1730,10 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1740,15 +1741,15 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1756,13 +1757,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" t="s">
         <v>61</v>
-      </c>
-      <c r="D35" t="s">
-        <v>62</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1770,13 +1771,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F36">
         <v>0</v>

</xml_diff>

<commit_message>
fix cotillion setup indicator
</commit_message>
<xml_diff>
--- a/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
+++ b/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\botc\botc_other\all_hat_and_no_cattle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61DCA3E-7564-4B1B-B508-6B7957AE684A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9030B8DE-313A-4272-A09C-55A0491E8A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1172,7 +1172,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,7 +1707,7 @@
         <v>54</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
messiah night order is after evil
</commit_message>
<xml_diff>
--- a/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
+++ b/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\botc\botc_other\all_hat_and_no_cattle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E312A6-C430-4AAD-A478-3C911AB218FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB0DF1C-B340-4458-8F6E-40CD1C8A18C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1171,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,10 +1258,10 @@
         <v>72</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1281,10 +1281,10 @@
         <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>10</v>
+        <v>95</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1330,7 +1330,7 @@
         <v>75</v>
       </c>
       <c r="I8" t="s">
-        <v>95</v>
+        <v>18</v>
       </c>
       <c r="J8" t="s">
         <v>73</v>
@@ -1356,7 +1356,7 @@
         <v>74</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="J9" t="s">
         <v>73</v>
@@ -1382,7 +1382,7 @@
         <v>74</v>
       </c>
       <c r="I10" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="J10" t="s">
         <v>73</v>
@@ -1408,7 +1408,7 @@
         <v>72</v>
       </c>
       <c r="I11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J11" t="s">
         <v>73</v>
@@ -1428,7 +1428,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="J12" t="s">
         <v>73</v>
@@ -1445,10 +1445,10 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J14" t="s">
         <v>74</v>
@@ -1482,10 +1482,10 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="J15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J16" t="s">
         <v>73</v>
@@ -1522,7 +1522,7 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="J17" t="s">
         <v>73</v>
@@ -1533,10 +1533,10 @@
         <v>39</v>
       </c>
       <c r="I18" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J18" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
revert previous, messiah before nightmare
</commit_message>
<xml_diff>
--- a/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
+++ b/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\botc\botc_other\all_hat_and_no_cattle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB0DF1C-B340-4458-8F6E-40CD1C8A18C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D9DE1F-A947-4F4D-9615-EC33582BA352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1172,7 +1172,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I5" sqref="I5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,10 +1258,10 @@
         <v>72</v>
       </c>
       <c r="I5" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1281,10 +1281,10 @@
         <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1307,10 +1307,10 @@
         <v>71</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="J7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1330,10 +1330,10 @@
         <v>75</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1356,7 +1356,7 @@
         <v>74</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="J9" t="s">
         <v>73</v>
@@ -1382,7 +1382,7 @@
         <v>74</v>
       </c>
       <c r="I10" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="J10" t="s">
         <v>73</v>
@@ -1408,7 +1408,7 @@
         <v>72</v>
       </c>
       <c r="I11" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="J11" t="s">
         <v>73</v>
@@ -1428,7 +1428,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J12" t="s">
         <v>73</v>
@@ -1445,10 +1445,10 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J14" t="s">
         <v>74</v>
@@ -1482,10 +1482,10 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="J15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J16" t="s">
         <v>73</v>
@@ -1522,7 +1522,7 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J17" t="s">
         <v>73</v>
@@ -1533,10 +1533,10 @@
         <v>39</v>
       </c>
       <c r="I18" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lumpus does not see grim
</commit_message>
<xml_diff>
--- a/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
+++ b/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\botc\botc_other\all_hat_and_no_cattle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDB2DD1-3834-4BE5-A969-63C6CDE1598D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17413C37-8475-4212-A8FE-6AF03D592ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -289,9 +289,6 @@
     <t>Each night*, choose a player to die. One of your minions is a non-listed (minion) role. A good player might learn from which script.</t>
   </si>
   <si>
-    <t>Each night*, see the Grimoire and choose a player to die, even if they might have survived for some reason. After your first kill, your target must neighbour a dead player.</t>
-  </si>
-  <si>
     <t>Each day, visit the storyteller and answer a yes/no question. In return you receive a piece of information, which is true if you answered correctly.</t>
   </si>
   <si>
@@ -310,9 +307,6 @@
     <t>On your first day, publicly choose 4 players (not yourself or travelers). At night you learn how many different character types they were.</t>
   </si>
   <si>
-    <t>When your exile is called for, visit the storyteller privately and choose a number. If exactly that many players vote, everyone who voted dies.</t>
-  </si>
-  <si>
     <t>If a Lemming dies, so do all other Lemmings. When Lemmings die, a dead minion might regain their ability for one day and night.</t>
   </si>
   <si>
@@ -332,6 +326,12 @@
   </si>
   <si>
     <t>Revives tonight</t>
+  </si>
+  <si>
+    <t>When your exile is called for, visit the storyteller privately and choose a number. If exactly that many players vote (not including you) everyone who voted dies.</t>
+  </si>
+  <si>
+    <t>Each night*, choose a player to die, even if they might have survived for some reason. After your first kill, your target must neighbour a dead player.</t>
   </si>
 </sst>
 </file>
@@ -1174,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,7 +1310,7 @@
         <v>71</v>
       </c>
       <c r="I7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J7" t="s">
         <v>73</v>
@@ -1321,7 +1321,7 @@
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1347,7 +1347,7 @@
         <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1370,7 +1370,7 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
@@ -1396,7 +1396,7 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" t="s">
         <v>31</v>
@@ -1445,7 +1445,7 @@
         <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1482,7 +1482,7 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1607,7 +1607,7 @@
         <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D22" t="s">
         <v>48</v>
@@ -1635,7 +1635,7 @@
         <v>80</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1643,13 +1643,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1660,7 +1660,7 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
         <v>67</v>
@@ -1721,7 +1721,7 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="D31" t="s">
         <v>54</v>
@@ -1735,7 +1735,7 @@
         <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D32" t="s">
         <v>54</v>
@@ -1754,7 +1754,7 @@
         <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F34">
         <v>0</v>

</xml_diff>

<commit_message>
Update All Hat And No Cattle.xlsx
minor
</commit_message>
<xml_diff>
--- a/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
+++ b/all_hat_and_no_cattle/All Hat And No Cattle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\botc\botc_other\all_hat_and_no_cattle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17413C37-8475-4212-A8FE-6AF03D592ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C885D5-0638-4E0F-82A4-976E3F210A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="102">
   <si>
     <t>All Hat And No Cattle</t>
   </si>
@@ -187,9 +187,6 @@
     <t>Siren</t>
   </si>
   <si>
-    <t>Each time you are nominated by an opposing player, they become drunk, even if you are dead.</t>
-  </si>
-  <si>
     <t>demon</t>
   </si>
   <si>
@@ -235,9 +232,6 @@
     <t>Runculus</t>
   </si>
   <si>
-    <t>Clockwise, Anticlockwise, No ability, Dead</t>
-  </si>
-  <si>
     <t>Cannot die, Drunk</t>
   </si>
   <si>
@@ -262,12 +256,6 @@
     <t>Ability - first night.</t>
   </si>
   <si>
-    <t>Any player (not yourself) who votes when you are nominated cannot die tonight, and one is drunk tonight.</t>
-  </si>
-  <si>
-    <t>On a tied nomination vote, two (or more) players are placed on the block. If so, at the end of the day, you choose which one of them is executed.</t>
-  </si>
-  <si>
     <t>If executed whilst dead, wake for new character choice.</t>
   </si>
   <si>
@@ -280,9 +268,6 @@
     <t>If a player is nominated and executed and you did not vote on their nomination, something bad might happen to your team. You survive execution.</t>
   </si>
   <si>
-    <t>The first time you are chosen at night by an opposing player, their ability malfunctions; the choice is redirected (without warning) at a new player of your choice.</t>
-  </si>
-  <si>
     <t>On your first day, visit the storyteller and choose two good characters. When either dies, you wake at night to learn that one (or both) died.</t>
   </si>
   <si>
@@ -292,9 +277,6 @@
     <t>Each day, visit the storyteller and answer a yes/no question. In return you receive a piece of information, which is true if you answered correctly.</t>
   </si>
   <si>
-    <t>On your first night, choose clockwise or anticlockwise. Once per game, at night*, along neighbouring alive players in that direction, choose if the furthest two from you die. The demon is drunk that night.</t>
-  </si>
-  <si>
     <t>Once per game, at night, choose a player (not travelers). If you choose a player of the same alignment or a demon, nothing happens. Otherwise, swap characters.</t>
   </si>
   <si>
@@ -310,9 +292,6 @@
     <t>If a Lemming dies, so do all other Lemmings. When Lemmings die, a dead minion might regain their ability for one day and night.</t>
   </si>
   <si>
-    <t>Each night*, choose a player to die. If you self-kill, and the living outnumber the dead, then minions choose a new evil hox and you become good. You don't learn bluffs or minions. Minions know you and learn bluffs.</t>
-  </si>
-  <si>
     <t>Nightmare</t>
   </si>
   <si>
@@ -332,6 +311,33 @@
   </si>
   <si>
     <t>Each night*, choose a player to die, even if they might have survived for some reason. After your first kill, your target must neighbour a dead player.</t>
+  </si>
+  <si>
+    <t>On a tied nomination vote, two (or more) players are placed on the block. At the end of the day, you choose which one of them is executed.</t>
+  </si>
+  <si>
+    <t>Enchanter</t>
+  </si>
+  <si>
+    <t>Enchanted</t>
+  </si>
+  <si>
+    <t>If you are chosen at night by a minion, their ability malfunctions; the choice is redirected (without warning) at a new player of your choice.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If a player targets the Enchanter, they become enchanted until targeted by another player. Enchanted players register as the Enchanter. </t>
+  </si>
+  <si>
+    <t>If you are nominated by an opposing player, they become drunk, even if you are dead.</t>
+  </si>
+  <si>
+    <t>Dead, On the block</t>
+  </si>
+  <si>
+    <t>Each night*, choose a player to die. Once per game, instead, choose to kill all players who were on the block today</t>
+  </si>
+  <si>
+    <t>Other players who voted on your exile today cannot die tonight (if you are not exiled), and one is drunk tonight.</t>
   </si>
 </sst>
 </file>
@@ -1172,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1232,13 +1238,13 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1258,13 +1264,13 @@
         <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s">
         <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1287,7 +1293,7 @@
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1307,13 +1313,13 @@
         <v>23</v>
       </c>
       <c r="H7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" t="s">
         <v>71</v>
-      </c>
-      <c r="I7" t="s">
-        <v>93</v>
-      </c>
-      <c r="J7" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1321,7 +1327,7 @@
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1330,13 +1336,13 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s">
         <v>18</v>
       </c>
       <c r="J8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1344,10 +1350,10 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" t="s">
         <v>83</v>
-      </c>
-      <c r="D9" t="s">
-        <v>89</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1356,13 +1362,13 @@
         <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1370,7 +1376,7 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
@@ -1382,13 +1388,13 @@
         <v>29</v>
       </c>
       <c r="H10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I10" t="s">
         <v>30</v>
       </c>
       <c r="J10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1396,7 +1402,7 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
         <v>31</v>
@@ -1408,13 +1414,13 @@
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I11" t="s">
         <v>23</v>
       </c>
       <c r="J11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1422,7 +1428,7 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
         <v>31</v>
@@ -1434,7 +1440,7 @@
         <v>32</v>
       </c>
       <c r="J12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1442,10 +1448,10 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1454,7 +1460,7 @@
         <v>29</v>
       </c>
       <c r="J13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1462,7 +1468,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
         <v>31</v>
@@ -1474,7 +1480,7 @@
         <v>27</v>
       </c>
       <c r="J14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1482,7 +1488,7 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1491,19 +1497,10 @@
         <v>11</v>
       </c>
       <c r="J15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" t="s">
-        <v>68</v>
-      </c>
       <c r="F16">
         <v>0</v>
       </c>
@@ -1511,7 +1508,7 @@
         <v>16</v>
       </c>
       <c r="J16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1519,7 +1516,7 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
         <v>37</v>
@@ -1531,7 +1528,7 @@
         <v>38</v>
       </c>
       <c r="J17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1542,7 +1539,7 @@
         <v>33</v>
       </c>
       <c r="J18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1553,7 +1550,7 @@
         <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1587,7 +1584,7 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
@@ -1607,7 +1604,7 @@
         <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D22" t="s">
         <v>48</v>
@@ -1619,7 +1616,7 @@
         <v>20</v>
       </c>
       <c r="J22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1632,10 +1629,10 @@
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1643,13 +1640,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1657,13 +1654,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1674,7 +1671,7 @@
         <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
@@ -1685,18 +1682,18 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1707,10 +1704,10 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1718,13 +1715,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1732,13 +1729,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
         <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1746,15 +1743,15 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1762,13 +1759,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1776,15 +1773,29 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D36" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>58</v>
       </c>
-      <c r="F36">
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37">
         <v>0</v>
       </c>
     </row>

</xml_diff>